<commit_message>
Object_reading update (and ge!!!!)
</commit_message>
<xml_diff>
--- a/I2_Gant.xlsx
+++ b/I2_Gant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB59F1BF-C6D1-406D-B6DF-6865631D696F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706A8FAD-E939-4DC1-BDBA-B1D6A6946059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>CRONOGRAMA I2</t>
   </si>
   <si>
-    <t>Desglose</t>
-  </si>
-  <si>
     <t>TAREAS</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>Fernando Mijangos Varas</t>
+  </si>
+  <si>
+    <t>DESGLOSE</t>
   </si>
 </sst>
 </file>
@@ -718,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -861,19 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -900,6 +888,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,7 +1234,7 @@
   <dimension ref="A1:Y56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1241,7 +1247,7 @@
     <col min="26" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -1270,20 +1276,20 @@
       <c r="X1" s="46"/>
       <c r="Y1" s="47"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+    <row r="2" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="54" t="s">
+      <c r="D2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="43" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="43" t="s">
-        <v>4</v>
       </c>
       <c r="G2" s="43"/>
       <c r="H2" s="43"/>
@@ -1305,50 +1311,50 @@
       <c r="X2" s="43"/>
       <c r="Y2" s="44"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" s="50"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="53"/>
+    <row r="3" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="43"/>
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
       <c r="J3" s="43"/>
       <c r="K3" s="43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L3" s="43"/>
       <c r="M3" s="43"/>
       <c r="N3" s="43"/>
       <c r="O3" s="43"/>
       <c r="P3" s="43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q3" s="43"/>
       <c r="R3" s="43"/>
       <c r="S3" s="43"/>
       <c r="T3" s="43"/>
       <c r="U3" s="43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V3" s="43"/>
       <c r="W3" s="43"/>
       <c r="X3" s="43"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="56"/>
+    <row r="4" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -1413,19 +1419,19 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="1"/>
@@ -1450,23 +1456,23 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1489,21 +1495,21 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1526,21 +1532,21 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="12">
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1563,21 +1569,21 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="12">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1600,24 +1606,24 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="12">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1639,24 +1645,24 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="12">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1678,25 +1684,25 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="12">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1717,27 +1723,27 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="12">
         <v>7</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1758,23 +1764,23 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="14">
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1795,26 +1801,26 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="14">
         <v>2</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1834,26 +1840,26 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="14">
         <v>3</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1873,24 +1879,24 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="14">
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1910,26 +1916,26 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="14">
         <v>5</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1946,22 +1952,22 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1969,7 +1975,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1988,17 +1994,17 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="8">
         <v>2</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -2006,60 +2012,60 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Y20" s="2"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="8">
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2067,7 +2073,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -2086,17 +2092,17 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="8">
         <v>4</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2104,10 +2110,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -2125,17 +2131,17 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="8">
         <v>5</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2143,10 +2149,10 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -2164,17 +2170,17 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="8">
         <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2182,10 +2188,10 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -2203,16 +2209,16 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="16">
         <v>1</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2220,7 +2226,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2240,16 +2246,16 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="18">
         <v>1</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2257,7 +2263,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2277,16 +2283,16 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="18">
         <v>2</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2294,10 +2300,10 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2316,16 +2322,16 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="18">
         <v>3</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2334,10 +2340,10 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -2355,16 +2361,16 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="18">
         <v>4</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2373,10 +2379,10 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -2394,16 +2400,16 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="20">
         <v>1</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2413,10 +2419,10 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -2433,16 +2439,16 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="22">
         <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2453,7 +2459,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2470,17 +2476,17 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="24">
         <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2490,7 +2496,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -2507,17 +2513,17 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" s="24">
         <v>2</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2527,7 +2533,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -2544,16 +2550,16 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="26">
         <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2565,7 +2571,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -2581,16 +2587,16 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="10">
         <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2602,7 +2608,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -2618,17 +2624,17 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A36" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="28">
         <v>1</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2639,7 +2645,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -2655,16 +2661,16 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" s="30">
         <v>1</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2677,7 +2683,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
@@ -2692,16 +2698,16 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A38" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" s="30">
         <v>2</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2714,10 +2720,10 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P38" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
@@ -2731,16 +2737,16 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A39" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" s="30">
         <v>3</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2754,7 +2760,7 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -2768,16 +2774,16 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A40" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" s="30">
         <v>4</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2791,10 +2797,10 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q40" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
@@ -2807,16 +2813,16 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A41" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" s="32">
         <v>1</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2832,7 +2838,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
@@ -2844,16 +2850,16 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A42" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="32">
         <v>2</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2869,10 +2875,10 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S42" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
@@ -2883,17 +2889,17 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A43" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43" s="34">
         <v>1</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2905,10 +2911,10 @@
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P43" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -2922,17 +2928,17 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" s="34">
         <v>2</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2944,7 +2950,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
@@ -2959,17 +2965,17 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="34">
         <v>3</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -2982,7 +2988,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -2996,17 +3002,17 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" s="34">
         <v>4</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -3019,10 +3025,10 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q46" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
@@ -3035,17 +3041,17 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" s="34">
         <v>5</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -3059,10 +3065,10 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R47" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
@@ -3074,17 +3080,17 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" s="34">
         <v>6</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -3098,10 +3104,10 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R48" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
@@ -3113,17 +3119,17 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A49" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" s="34">
         <v>7</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -3138,10 +3144,10 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S49" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
@@ -3152,17 +3158,17 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A50" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="34">
         <v>8</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -3178,7 +3184,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
@@ -3189,17 +3195,17 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A51" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51" s="34">
         <v>9</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -3215,7 +3221,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
@@ -3226,19 +3232,19 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A52" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B52" s="22">
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -3263,19 +3269,19 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A53" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" s="36">
         <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="36"/>
@@ -3300,13 +3306,13 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A54" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B54" s="38">
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -3333,16 +3339,16 @@
     </row>
     <row r="55" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="41">
         <v>1</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -3365,7 +3371,7 @@
       <c r="W55" s="4"/>
       <c r="X55" s="4"/>
       <c r="Y55" s="42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3402,27 +3408,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="60" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="63" t="s">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="60" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>

</xml_diff>